<commit_message>
Further work with PP graphics
</commit_message>
<xml_diff>
--- a/results/palaepaphos/data/grain_PP.xlsx
+++ b/results/palaepaphos/data/grain_PP.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uine\Documents\R\MB\results\palaepaphos\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R\MB\results\palaepaphos\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9DD9456-4BCC-47D5-8A34-16F23D2C5666}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="105" windowWidth="17715" windowHeight="15495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="105" windowWidth="17715" windowHeight="15495"/>
   </bookViews>
   <sheets>
     <sheet name="Particle-size-final" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="58">
   <si>
     <t>Result Above 2000.000 µm</t>
   </si>
@@ -43,12 +42,6 @@
   </si>
   <si>
     <t>d (0.9)</t>
-  </si>
-  <si>
-    <t>PP-1</t>
-  </si>
-  <si>
-    <t>PP-1 - Average</t>
   </si>
   <si>
     <t>PP-10</t>
@@ -117,42 +110,6 @@
     <t>PP-19 - Average</t>
   </si>
   <si>
-    <t>PP-2</t>
-  </si>
-  <si>
-    <t>PP-2 - Average</t>
-  </si>
-  <si>
-    <t>PP-3</t>
-  </si>
-  <si>
-    <t>PP-3 - Average</t>
-  </si>
-  <si>
-    <t>PP-4</t>
-  </si>
-  <si>
-    <t>PP-4 - Average</t>
-  </si>
-  <si>
-    <t>PP-5</t>
-  </si>
-  <si>
-    <t>PP-5 - Average</t>
-  </si>
-  <si>
-    <t>PP-6</t>
-  </si>
-  <si>
-    <t>PP-6 - Average</t>
-  </si>
-  <si>
-    <t>PP-7</t>
-  </si>
-  <si>
-    <t>PP-7 - Average</t>
-  </si>
-  <si>
     <t>PP-9</t>
   </si>
   <si>
@@ -171,12 +128,6 @@
     <t>Sand</t>
   </si>
   <si>
-    <t>PP-8</t>
-  </si>
-  <si>
-    <t>PP-8 - Average</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -184,30 +135,6 @@
   </si>
   <si>
     <t>Type</t>
-  </si>
-  <si>
-    <t>Hadjuabudllah l1</t>
-  </si>
-  <si>
-    <t>Hadjuabudllah l2</t>
-  </si>
-  <si>
-    <t>soil layer 1</t>
-  </si>
-  <si>
-    <t>soil layer 2</t>
-  </si>
-  <si>
-    <t>soil layer 3</t>
-  </si>
-  <si>
-    <t>Laona soil l1</t>
-  </si>
-  <si>
-    <t>Laona soil l2</t>
-  </si>
-  <si>
-    <t>Laona soil l3</t>
   </si>
   <si>
     <t>mudbrick</t>
@@ -221,16 +148,74 @@
   <si>
     <t>LA54:7</t>
   </si>
+  <si>
+    <t>soil</t>
+  </si>
+  <si>
+    <t>S-1</t>
+  </si>
+  <si>
+    <t>S-1 - Average</t>
+  </si>
+  <si>
+    <t>S-2</t>
+  </si>
+  <si>
+    <t>S-2 - Average</t>
+  </si>
+  <si>
+    <t>S-3</t>
+  </si>
+  <si>
+    <t>S-3 - Average</t>
+  </si>
+  <si>
+    <t>S-4</t>
+  </si>
+  <si>
+    <t>S-4 - Average</t>
+  </si>
+  <si>
+    <t>S-5</t>
+  </si>
+  <si>
+    <t>S-5 - Average</t>
+  </si>
+  <si>
+    <t>S-6</t>
+  </si>
+  <si>
+    <t>S-6 - Average</t>
+  </si>
+  <si>
+    <t>S-7</t>
+  </si>
+  <si>
+    <t>S-7 - Average</t>
+  </si>
+  <si>
+    <t>S-8</t>
+  </si>
+  <si>
+    <t>S-8 - Average</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -271,14 +256,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,11 +479,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DI83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="B33" sqref="B2:B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -511,25 +497,25 @@
   <sheetData>
     <row r="1" spans="1:113" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>0</v>
@@ -854,14 +840,14 @@
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
+      <c r="B2" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>55</v>
+        <v>41</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="E2" s="2">
         <v>0.97699999999999998</v>
@@ -1196,13 +1182,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>55</v>
+        <v>41</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="E3" s="2">
         <v>1.0309999999999999</v>
@@ -1537,13 +1523,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>55</v>
+        <v>41</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="E4" s="2">
         <v>1.06</v>
@@ -1878,13 +1864,13 @@
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>55</v>
+        <v>41</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="E5" s="2">
         <v>1.0229999999999999</v>
@@ -2219,13 +2205,13 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="E6" s="2">
         <v>23.699000000000002</v>
@@ -2560,13 +2546,13 @@
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="E7" s="2">
         <v>4.5149999999999997</v>
@@ -2901,13 +2887,13 @@
         <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="E8" s="2">
         <v>3.7570000000000001</v>
@@ -3242,13 +3228,13 @@
         <v>2</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="E9" s="2">
         <v>10.657</v>
@@ -3583,13 +3569,13 @@
         <v>3</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="E10" s="2">
         <v>0.998</v>
@@ -3924,13 +3910,13 @@
         <v>3</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="E11" s="2">
         <v>0.64800000000000002</v>
@@ -4265,13 +4251,13 @@
         <v>3</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="E12" s="2">
         <v>0.48799999999999999</v>
@@ -4606,13 +4592,13 @@
         <v>3</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="E13" s="2">
         <v>0.71099999999999997</v>
@@ -4947,13 +4933,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="E14" s="2">
         <v>3.5630000000000002</v>
@@ -5288,13 +5274,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="E15" s="2">
         <v>3.5459999999999998</v>
@@ -5629,13 +5615,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="E16" s="2">
         <v>3.5459999999999998</v>
@@ -5970,13 +5956,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="E17" s="2">
         <v>3.552</v>
@@ -6311,13 +6297,13 @@
         <v>5</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="E18" s="2">
         <v>1.696</v>
@@ -6652,13 +6638,13 @@
         <v>5</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="E19" s="2">
         <v>0</v>
@@ -6993,13 +6979,13 @@
         <v>5</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="E20" s="2">
         <v>0</v>
@@ -7334,13 +7320,13 @@
         <v>5</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="E21" s="2">
         <v>0.56499999999999995</v>
@@ -7675,13 +7661,13 @@
         <v>6</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="E22" s="2">
         <v>3.597</v>
@@ -8016,13 +8002,13 @@
         <v>6</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="E23" s="2">
         <v>4.2469999999999999</v>
@@ -8357,13 +8343,13 @@
         <v>6</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="E24" s="2">
         <v>4.6900000000000004</v>
@@ -8698,13 +8684,13 @@
         <v>6</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="E25" s="2">
         <v>4.1779999999999999</v>
@@ -9039,13 +9025,13 @@
         <v>7</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="E26" s="2">
         <v>12.977</v>
@@ -9380,13 +9366,13 @@
         <v>7</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="E27" s="2">
         <v>13.641999999999999</v>
@@ -9721,13 +9707,13 @@
         <v>7</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="E28" s="2">
         <v>14.59</v>
@@ -10062,13 +10048,13 @@
         <v>7</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>59</v>
-      </c>
       <c r="D29" s="4" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="E29" s="2">
         <v>13.736000000000001</v>
@@ -10403,13 +10389,13 @@
         <v>8</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="E30" s="2">
         <v>11.257</v>
@@ -10744,13 +10730,13 @@
         <v>8</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="E31" s="2">
         <v>12.086</v>
@@ -11085,13 +11071,13 @@
         <v>8</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="E32" s="2">
         <v>12.391999999999999</v>
@@ -11426,13 +11412,13 @@
         <v>8</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="E33" s="2">
         <v>11.911</v>
@@ -11767,13 +11753,13 @@
         <v>9</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E34" s="2">
         <v>1.552</v>
@@ -12108,13 +12094,13 @@
         <v>9</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E35" s="2">
         <v>1.821</v>
@@ -12449,13 +12435,13 @@
         <v>9</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E36" s="2">
         <v>1.821</v>
@@ -12790,13 +12776,13 @@
         <v>9</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E37" s="2">
         <v>1.732</v>
@@ -13131,13 +13117,13 @@
         <v>10</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E38" s="2">
         <v>0.81299999999999994</v>
@@ -13472,13 +13458,13 @@
         <v>10</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E39" s="2">
         <v>0.871</v>
@@ -13813,13 +13799,13 @@
         <v>10</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E40" s="2">
         <v>0.86</v>
@@ -14154,13 +14140,13 @@
         <v>10</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E41" s="2">
         <v>0.84799999999999998</v>
@@ -14495,13 +14481,13 @@
         <v>11</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E42" s="2">
         <v>1.1559999999999999</v>
@@ -14836,13 +14822,13 @@
         <v>11</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E43" s="2">
         <v>1.329</v>
@@ -15177,13 +15163,13 @@
         <v>11</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E44" s="2">
         <v>1.419</v>
@@ -15518,13 +15504,13 @@
         <v>11</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E45" s="2">
         <v>1.3009999999999999</v>
@@ -15859,13 +15845,13 @@
         <v>12</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E46" s="2">
         <v>10.76</v>
@@ -16200,13 +16186,13 @@
         <v>12</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E47" s="2">
         <v>11.819000000000001</v>
@@ -16541,13 +16527,13 @@
         <v>12</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E48" s="2">
         <v>12.074</v>
@@ -16882,13 +16868,13 @@
         <v>12</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E49" s="2">
         <v>11.551</v>
@@ -17223,13 +17209,13 @@
         <v>13</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E50" s="2">
         <v>2.1819999999999999</v>
@@ -17564,13 +17550,13 @@
         <v>13</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E51" s="2">
         <v>2.677</v>
@@ -17905,13 +17891,13 @@
         <v>13</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E52" s="2">
         <v>2.8610000000000002</v>
@@ -18246,13 +18232,13 @@
         <v>13</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E53" s="2">
         <v>2.573</v>
@@ -18587,13 +18573,13 @@
         <v>13</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E54" s="2">
         <v>3.758</v>
@@ -18928,13 +18914,13 @@
         <v>13</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E55" s="2">
         <v>3.7730000000000001</v>
@@ -19269,13 +19255,13 @@
         <v>13</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E56" s="2">
         <v>3.944</v>
@@ -19610,13 +19596,13 @@
         <v>13</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E57" s="2">
         <v>4.1230000000000002</v>
@@ -19951,13 +19937,13 @@
         <v>13</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E58" s="2">
         <v>3.9529999999999998</v>
@@ -20292,13 +20278,13 @@
         <v>13</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E59" s="2">
         <v>3.91</v>
@@ -20633,13 +20619,13 @@
         <v>14</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E60" s="2">
         <v>0.872</v>
@@ -20974,13 +20960,13 @@
         <v>14</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E61" s="2">
         <v>0.93</v>
@@ -21315,13 +21301,13 @@
         <v>14</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E62" s="2">
         <v>1.032</v>
@@ -21656,13 +21642,13 @@
         <v>14</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E63" s="2">
         <v>0.94499999999999995</v>
@@ -21997,13 +21983,13 @@
         <v>15</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E64" s="2">
         <v>8.8829999999999991</v>
@@ -22338,13 +22324,13 @@
         <v>15</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E65" s="2">
         <v>10.404999999999999</v>
@@ -22679,13 +22665,13 @@
         <v>15</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E66" s="2">
         <v>9.86</v>
@@ -23020,13 +23006,13 @@
         <v>15</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E67" s="2">
         <v>9.7159999999999993</v>
@@ -23361,13 +23347,13 @@
         <v>16</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E68" s="2">
         <v>0.88700000000000001</v>
@@ -23702,13 +23688,13 @@
         <v>16</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E69" s="2">
         <v>0.91100000000000003</v>
@@ -24043,13 +24029,13 @@
         <v>16</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E70" s="2">
         <v>0.97699999999999998</v>
@@ -24384,13 +24370,13 @@
         <v>16</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E71" s="2">
         <v>0.92500000000000004</v>
@@ -24725,13 +24711,13 @@
         <v>17</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E72" s="2">
         <v>1.359</v>
@@ -25066,13 +25052,13 @@
         <v>17</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E73" s="2">
         <v>1.4990000000000001</v>
@@ -25407,13 +25393,13 @@
         <v>17</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E74" s="2">
         <v>1.5</v>
@@ -25748,13 +25734,13 @@
         <v>17</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E75" s="2">
         <v>1.4530000000000001</v>
@@ -26089,13 +26075,13 @@
         <v>18</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E76" s="2">
         <v>1.054</v>
@@ -26430,13 +26416,13 @@
         <v>18</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E77" s="2">
         <v>1.095</v>
@@ -26771,13 +26757,13 @@
         <v>18</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E78" s="2">
         <v>1.1879999999999999</v>
@@ -27112,13 +27098,13 @@
         <v>18</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E79" s="2">
         <v>1.1120000000000001</v>
@@ -27453,13 +27439,13 @@
         <v>19</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E80" s="2">
         <v>1.589</v>
@@ -27794,13 +27780,13 @@
         <v>19</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E81" s="2">
         <v>1.8740000000000001</v>
@@ -28135,13 +28121,13 @@
         <v>19</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E82" s="2">
         <v>1.708</v>
@@ -28476,13 +28462,13 @@
         <v>19</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E83" s="2">
         <v>1.7230000000000001</v>
@@ -28813,10 +28799,10 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:DI83">
+  <sortState ref="A2:DI83">
     <sortCondition ref="A2:A83"/>
   </sortState>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>

</xml_diff>